<commit_message>
Updating with most recent version
</commit_message>
<xml_diff>
--- a/data/Results.xlsx
+++ b/data/Results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -474,231 +474,35 @@
           <t>Away LB Return</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>Home Bet</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>Away Bet</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>CLE</t>
+          <t>TOR</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>SAC</t>
+          <t>NYK</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>-170</v>
+        <v>200</v>
       </c>
       <c r="D2" t="n">
-        <v>142</v>
+        <v>-245</v>
       </c>
       <c r="E2" t="n">
-        <v>0.6879406795897915</v>
+        <v>0.3507480227274955</v>
       </c>
       <c r="F2" t="n">
-        <v>0.3120544181573381</v>
+        <v>0.6495308864939859</v>
       </c>
       <c r="G2" t="n">
-        <v>1.319990287790425</v>
+        <v>-9.775593181751347</v>
       </c>
       <c r="H2" t="n">
-        <v>1.005795337321175</v>
-      </c>
-      <c r="I2" t="n">
-        <v>0</v>
-      </c>
-      <c r="J2" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>PHI</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>DAL</t>
-        </is>
-      </c>
-      <c r="C3" t="n">
-        <v>136</v>
-      </c>
-      <c r="D3" t="n">
-        <v>-162</v>
-      </c>
-      <c r="E3" t="n">
-        <v>0.7332958622699053</v>
-      </c>
-      <c r="F3" t="n">
-        <v>0.2666240633108422</v>
-      </c>
-      <c r="G3" t="n">
-        <v>61.25782349569764</v>
-      </c>
-      <c r="H3" t="n">
-        <v>-18.29855801308094</v>
-      </c>
-      <c r="I3" t="n">
-        <v>0.7332958622699053</v>
-      </c>
-      <c r="J3" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>CHA</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>LAL</t>
-        </is>
-      </c>
-      <c r="C4" t="n">
-        <v>525</v>
-      </c>
-      <c r="D4" t="n">
-        <v>-750</v>
-      </c>
-      <c r="E4" t="n">
-        <v>0.2977994568870492</v>
-      </c>
-      <c r="F4" t="n">
-        <v>0.7021764238743191</v>
-      </c>
-      <c r="G4" t="n">
-        <v>54.87466055440578</v>
-      </c>
-      <c r="H4" t="n">
-        <v>-66.5243686596375</v>
-      </c>
-      <c r="I4" t="n">
-        <v>0.2977994568870492</v>
-      </c>
-      <c r="J4" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>BKN</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>GSW</t>
-        </is>
-      </c>
-      <c r="C5" t="n">
-        <v>-102</v>
-      </c>
-      <c r="D5" t="n">
-        <v>-118</v>
-      </c>
-      <c r="E5" t="n">
-        <v>0.6076707360039044</v>
-      </c>
-      <c r="F5" t="n">
-        <v>0.3923499865173703</v>
-      </c>
-      <c r="G5" t="n">
-        <v>10.44067516940068</v>
-      </c>
-      <c r="H5" t="n">
-        <v>-15.22021567779851</v>
-      </c>
-      <c r="I5" t="n">
-        <v>0</v>
-      </c>
-      <c r="J5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>ATL</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>LAC</t>
-        </is>
-      </c>
-      <c r="C6" t="n">
-        <v>150</v>
-      </c>
-      <c r="D6" t="n">
-        <v>-180</v>
-      </c>
-      <c r="E6" t="n">
-        <v>0.3860438792319744</v>
-      </c>
-      <c r="F6" t="n">
-        <v>0.6139791208342429</v>
-      </c>
-      <c r="G6" t="n">
-        <v>-15.98903019200641</v>
-      </c>
-      <c r="H6" t="n">
-        <v>-35.06343869712241</v>
-      </c>
-      <c r="I6" t="n">
-        <v>0</v>
-      </c>
-      <c r="J6" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>NOP</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>TOR</t>
-        </is>
-      </c>
-      <c r="C7" t="n">
-        <v>-575</v>
-      </c>
-      <c r="D7" t="n">
-        <v>425</v>
-      </c>
-      <c r="E7" t="n">
-        <v>0.7428449900324272</v>
-      </c>
-      <c r="F7" t="n">
-        <v>0.2570549654412338</v>
-      </c>
-      <c r="G7" t="n">
-        <v>-18.66602290923681</v>
-      </c>
-      <c r="H7" t="n">
-        <v>57.28285931576709</v>
-      </c>
-      <c r="I7" t="n">
-        <v>0</v>
-      </c>
-      <c r="J7" t="n">
-        <v>0.2570549654412338</v>
+        <v>-45.45454929892449</v>
       </c>
     </row>
   </sheetData>

</xml_diff>